<commit_message>
feat: Updated Planning (again)
</commit_message>
<xml_diff>
--- a/ext/planning/Planning_SolarSystem_et_FluidSimulation.xlsx
+++ b/ext/planning/Planning_SolarSystem_et_FluidSimulation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20412"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Atelier\3e annee\Vadi\Projet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ComtesseE1\Desktop\astral-simulation\ext\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D01D202-EA1F-459A-84D0-8B7EED65F8C3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A33B89C5-BB17-4846-9809-1E61FA082A9F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{3DB24536-05C8-427A-A68F-F968813ACFE6}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="56">
   <si>
     <t>11.11.2024
 Vadi/Schenk</t>
@@ -167,9 +167,6 @@
     <t>Calcul de la force de gravitation du soleil</t>
   </si>
   <si>
-    <t>Calcul de la rotation des astres</t>
-  </si>
-  <si>
     <t>Ajout de la rotation des astres</t>
   </si>
   <si>
@@ -183,9 +180,6 @@
   </si>
   <si>
     <t>Affichage des informations d'une planète</t>
-  </si>
-  <si>
-    <t>Liaison des informations</t>
   </si>
   <si>
     <t>Rajouter une fenêtre permettant d'implémenter de nouveaux astres</t>
@@ -265,7 +259,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -292,6 +286,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -537,14 +537,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -561,18 +558,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutre" xfId="1" builtinId="28"/>
@@ -902,170 +900,170 @@
   <sheetData>
     <row r="1" spans="1:109" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="B1" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="30" t="s">
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="34"/>
-      <c r="K1" s="35" t="s">
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="36"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="30" t="s">
+      <c r="L1" s="37"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="O1" s="31"/>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="32"/>
-      <c r="R1" s="30" t="s">
+      <c r="O1" s="39"/>
+      <c r="P1" s="39"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="S1" s="33"/>
-      <c r="T1" s="33"/>
-      <c r="U1" s="33"/>
-      <c r="V1" s="34"/>
-      <c r="W1" s="35" t="s">
+      <c r="S1" s="34"/>
+      <c r="T1" s="34"/>
+      <c r="U1" s="34"/>
+      <c r="V1" s="35"/>
+      <c r="W1" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="X1" s="36"/>
-      <c r="Y1" s="37"/>
-      <c r="Z1" s="30" t="s">
+      <c r="X1" s="37"/>
+      <c r="Y1" s="38"/>
+      <c r="Z1" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="AA1" s="31"/>
-      <c r="AB1" s="31"/>
-      <c r="AC1" s="32"/>
-      <c r="AD1" s="30" t="s">
+      <c r="AA1" s="39"/>
+      <c r="AB1" s="39"/>
+      <c r="AC1" s="40"/>
+      <c r="AD1" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="AE1" s="33"/>
-      <c r="AF1" s="33"/>
-      <c r="AG1" s="33"/>
-      <c r="AH1" s="34"/>
-      <c r="AI1" s="35" t="s">
+      <c r="AE1" s="34"/>
+      <c r="AF1" s="34"/>
+      <c r="AG1" s="34"/>
+      <c r="AH1" s="35"/>
+      <c r="AI1" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="AJ1" s="36"/>
-      <c r="AK1" s="37"/>
-      <c r="AL1" s="30" t="s">
+      <c r="AJ1" s="37"/>
+      <c r="AK1" s="38"/>
+      <c r="AL1" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="AM1" s="31"/>
-      <c r="AN1" s="31"/>
-      <c r="AO1" s="32"/>
-      <c r="AP1" s="30" t="s">
+      <c r="AM1" s="39"/>
+      <c r="AN1" s="39"/>
+      <c r="AO1" s="40"/>
+      <c r="AP1" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="AQ1" s="33"/>
-      <c r="AR1" s="33"/>
-      <c r="AS1" s="33"/>
-      <c r="AT1" s="34"/>
-      <c r="AU1" s="35" t="s">
+      <c r="AQ1" s="34"/>
+      <c r="AR1" s="34"/>
+      <c r="AS1" s="34"/>
+      <c r="AT1" s="35"/>
+      <c r="AU1" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="AV1" s="36"/>
-      <c r="AW1" s="37"/>
-      <c r="AX1" s="30" t="s">
+      <c r="AV1" s="37"/>
+      <c r="AW1" s="38"/>
+      <c r="AX1" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="AY1" s="31"/>
-      <c r="AZ1" s="31"/>
-      <c r="BA1" s="32"/>
-      <c r="BB1" s="30" t="s">
+      <c r="AY1" s="39"/>
+      <c r="AZ1" s="39"/>
+      <c r="BA1" s="40"/>
+      <c r="BB1" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="BC1" s="33"/>
-      <c r="BD1" s="33"/>
-      <c r="BE1" s="33"/>
-      <c r="BF1" s="34"/>
-      <c r="BG1" s="35" t="s">
+      <c r="BC1" s="34"/>
+      <c r="BD1" s="34"/>
+      <c r="BE1" s="34"/>
+      <c r="BF1" s="35"/>
+      <c r="BG1" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="BH1" s="36"/>
-      <c r="BI1" s="37"/>
-      <c r="BJ1" s="30" t="s">
+      <c r="BH1" s="37"/>
+      <c r="BI1" s="38"/>
+      <c r="BJ1" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="BK1" s="31"/>
-      <c r="BL1" s="31"/>
-      <c r="BM1" s="32"/>
-      <c r="BN1" s="30" t="s">
+      <c r="BK1" s="39"/>
+      <c r="BL1" s="39"/>
+      <c r="BM1" s="40"/>
+      <c r="BN1" s="33" t="s">
         <v>12</v>
       </c>
-      <c r="BO1" s="33"/>
-      <c r="BP1" s="33"/>
-      <c r="BQ1" s="33"/>
-      <c r="BR1" s="34"/>
-      <c r="BS1" s="35" t="s">
+      <c r="BO1" s="34"/>
+      <c r="BP1" s="34"/>
+      <c r="BQ1" s="34"/>
+      <c r="BR1" s="35"/>
+      <c r="BS1" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="BT1" s="36"/>
-      <c r="BU1" s="37"/>
-      <c r="BV1" s="30" t="s">
+      <c r="BT1" s="37"/>
+      <c r="BU1" s="38"/>
+      <c r="BV1" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="BW1" s="31"/>
-      <c r="BX1" s="31"/>
-      <c r="BY1" s="32"/>
-      <c r="BZ1" s="30" t="s">
+      <c r="BW1" s="39"/>
+      <c r="BX1" s="39"/>
+      <c r="BY1" s="40"/>
+      <c r="BZ1" s="33" t="s">
         <v>14</v>
       </c>
-      <c r="CA1" s="33"/>
-      <c r="CB1" s="33"/>
-      <c r="CC1" s="33"/>
-      <c r="CD1" s="34"/>
-      <c r="CE1" s="35" t="s">
+      <c r="CA1" s="34"/>
+      <c r="CB1" s="34"/>
+      <c r="CC1" s="34"/>
+      <c r="CD1" s="35"/>
+      <c r="CE1" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="CF1" s="36"/>
-      <c r="CG1" s="37"/>
-      <c r="CH1" s="30" t="s">
+      <c r="CF1" s="37"/>
+      <c r="CG1" s="38"/>
+      <c r="CH1" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="CI1" s="31"/>
-      <c r="CJ1" s="31"/>
-      <c r="CK1" s="32"/>
-      <c r="CL1" s="30" t="s">
+      <c r="CI1" s="39"/>
+      <c r="CJ1" s="39"/>
+      <c r="CK1" s="40"/>
+      <c r="CL1" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="CM1" s="33"/>
-      <c r="CN1" s="33"/>
-      <c r="CO1" s="33"/>
-      <c r="CP1" s="34"/>
-      <c r="CQ1" s="35" t="s">
+      <c r="CM1" s="34"/>
+      <c r="CN1" s="34"/>
+      <c r="CO1" s="34"/>
+      <c r="CP1" s="35"/>
+      <c r="CQ1" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="CR1" s="36"/>
-      <c r="CS1" s="37"/>
-      <c r="CT1" s="30" t="s">
+      <c r="CR1" s="37"/>
+      <c r="CS1" s="38"/>
+      <c r="CT1" s="33" t="s">
         <v>26</v>
       </c>
-      <c r="CU1" s="31"/>
-      <c r="CV1" s="31"/>
-      <c r="CW1" s="32"/>
-      <c r="CX1" s="30" t="s">
+      <c r="CU1" s="39"/>
+      <c r="CV1" s="39"/>
+      <c r="CW1" s="40"/>
+      <c r="CX1" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="CY1" s="33"/>
-      <c r="CZ1" s="33"/>
-      <c r="DA1" s="33"/>
-      <c r="DB1" s="34"/>
-      <c r="DC1" s="35" t="s">
+      <c r="CY1" s="34"/>
+      <c r="CZ1" s="34"/>
+      <c r="DA1" s="34"/>
+      <c r="DB1" s="35"/>
+      <c r="DC1" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="DD1" s="36"/>
-      <c r="DE1" s="37"/>
+      <c r="DD1" s="37"/>
+      <c r="DE1" s="38"/>
     </row>
     <row r="2" spans="1:109" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
@@ -1398,7 +1396,7 @@
     </row>
     <row r="3" spans="1:109" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B3" s="21"/>
       <c r="C3" s="21"/>
@@ -1511,7 +1509,7 @@
     </row>
     <row r="4" spans="1:109" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B4" s="12"/>
       <c r="C4" s="12"/>
@@ -1624,7 +1622,7 @@
     </row>
     <row r="5" spans="1:109" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>
@@ -1737,7 +1735,7 @@
     </row>
     <row r="6" spans="1:109" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
@@ -1850,7 +1848,7 @@
     </row>
     <row r="7" spans="1:109" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
@@ -1963,7 +1961,7 @@
     </row>
     <row r="8" spans="1:109" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
@@ -2076,7 +2074,7 @@
     </row>
     <row r="9" spans="1:109" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>
@@ -2189,7 +2187,7 @@
     </row>
     <row r="10" spans="1:109" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B10" s="12"/>
       <c r="C10" s="12"/>
@@ -2302,7 +2300,7 @@
     </row>
     <row r="11" spans="1:109" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12"/>
@@ -2415,7 +2413,7 @@
     </row>
     <row r="12" spans="1:109" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B12" s="12"/>
       <c r="C12" s="12"/>
@@ -2528,7 +2526,7 @@
     </row>
     <row r="13" spans="1:109" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="12"/>
@@ -2641,7 +2639,7 @@
     </row>
     <row r="14" spans="1:109" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B14" s="12"/>
       <c r="C14" s="12"/>
@@ -2754,7 +2752,7 @@
     </row>
     <row r="15" spans="1:109" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="20" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B15" s="24"/>
       <c r="C15" s="24"/>
@@ -2927,11 +2925,16 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="CL1:CP1"/>
-    <mergeCell ref="CQ1:CS1"/>
-    <mergeCell ref="CT1:CW1"/>
-    <mergeCell ref="CX1:DB1"/>
-    <mergeCell ref="DC1:DE1"/>
+    <mergeCell ref="AL1:AO1"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:V1"/>
+    <mergeCell ref="W1:Y1"/>
+    <mergeCell ref="Z1:AC1"/>
+    <mergeCell ref="AD1:AH1"/>
+    <mergeCell ref="AI1:AK1"/>
     <mergeCell ref="CH1:CK1"/>
     <mergeCell ref="AP1:AT1"/>
     <mergeCell ref="AU1:AW1"/>
@@ -2944,16 +2947,11 @@
     <mergeCell ref="BV1:BY1"/>
     <mergeCell ref="BZ1:CD1"/>
     <mergeCell ref="CE1:CG1"/>
-    <mergeCell ref="AL1:AO1"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:V1"/>
-    <mergeCell ref="W1:Y1"/>
-    <mergeCell ref="Z1:AC1"/>
-    <mergeCell ref="AD1:AH1"/>
-    <mergeCell ref="AI1:AK1"/>
+    <mergeCell ref="CL1:CP1"/>
+    <mergeCell ref="CQ1:CS1"/>
+    <mergeCell ref="CT1:CW1"/>
+    <mergeCell ref="CX1:DB1"/>
+    <mergeCell ref="DC1:DE1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2962,186 +2960,141 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74F55DC9-37A6-4B0F-B617-3DB57FA71D61}">
-  <dimension ref="A1:DE31"/>
+  <dimension ref="A1:CD29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="W17" sqref="W17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="109" width="4.7109375" customWidth="1"/>
+    <col min="2" max="82" width="4.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:109" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:82" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="40" t="s">
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38"/>
-      <c r="N1" s="40" t="s">
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="O1" s="39"/>
-      <c r="P1" s="39"/>
-      <c r="Q1" s="39"/>
-      <c r="R1" s="40" t="s">
+      <c r="L1" s="42"/>
+      <c r="M1" s="42"/>
+      <c r="N1" s="42"/>
+      <c r="O1" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="S1" s="40"/>
-      <c r="T1" s="40"/>
-      <c r="U1" s="40"/>
-      <c r="V1" s="40"/>
-      <c r="W1" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="X1" s="38"/>
-      <c r="Y1" s="38"/>
-      <c r="Z1" s="40" t="s">
+      <c r="P1" s="41"/>
+      <c r="Q1" s="41"/>
+      <c r="R1" s="41"/>
+      <c r="S1" s="41"/>
+      <c r="T1" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="AA1" s="39"/>
-      <c r="AB1" s="39"/>
-      <c r="AC1" s="39"/>
-      <c r="AD1" s="40" t="s">
+      <c r="U1" s="42"/>
+      <c r="V1" s="42"/>
+      <c r="W1" s="42"/>
+      <c r="X1" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="AE1" s="40"/>
-      <c r="AF1" s="40"/>
-      <c r="AG1" s="40"/>
-      <c r="AH1" s="40"/>
-      <c r="AI1" s="38" t="s">
-        <v>7</v>
-      </c>
-      <c r="AJ1" s="38"/>
-      <c r="AK1" s="38"/>
-      <c r="AL1" s="40" t="s">
+      <c r="Y1" s="41"/>
+      <c r="Z1" s="41"/>
+      <c r="AA1" s="41"/>
+      <c r="AB1" s="41"/>
+      <c r="AC1" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="AM1" s="39"/>
-      <c r="AN1" s="39"/>
-      <c r="AO1" s="39"/>
-      <c r="AP1" s="40" t="s">
+      <c r="AD1" s="42"/>
+      <c r="AE1" s="42"/>
+      <c r="AF1" s="42"/>
+      <c r="AG1" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="AQ1" s="40"/>
-      <c r="AR1" s="40"/>
-      <c r="AS1" s="40"/>
-      <c r="AT1" s="40"/>
-      <c r="AU1" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="AV1" s="38"/>
-      <c r="AW1" s="38"/>
-      <c r="AX1" s="40" t="s">
+      <c r="AH1" s="41"/>
+      <c r="AI1" s="41"/>
+      <c r="AJ1" s="41"/>
+      <c r="AK1" s="41"/>
+      <c r="AL1" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="AY1" s="39"/>
-      <c r="AZ1" s="39"/>
-      <c r="BA1" s="39"/>
-      <c r="BB1" s="40" t="s">
+      <c r="AM1" s="42"/>
+      <c r="AN1" s="42"/>
+      <c r="AO1" s="42"/>
+      <c r="AP1" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="BC1" s="40"/>
-      <c r="BD1" s="40"/>
-      <c r="BE1" s="40"/>
-      <c r="BF1" s="40"/>
-      <c r="BG1" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="BH1" s="38"/>
-      <c r="BI1" s="38"/>
-      <c r="BJ1" s="40" t="s">
+      <c r="AQ1" s="41"/>
+      <c r="AR1" s="41"/>
+      <c r="AS1" s="41"/>
+      <c r="AT1" s="41"/>
+      <c r="AU1" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="BK1" s="39"/>
-      <c r="BL1" s="39"/>
-      <c r="BM1" s="39"/>
-      <c r="BN1" s="40" t="s">
+      <c r="AV1" s="42"/>
+      <c r="AW1" s="42"/>
+      <c r="AX1" s="42"/>
+      <c r="AY1" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="BO1" s="40"/>
-      <c r="BP1" s="40"/>
-      <c r="BQ1" s="40"/>
-      <c r="BR1" s="40"/>
-      <c r="BS1" s="38" t="s">
-        <v>13</v>
-      </c>
-      <c r="BT1" s="38"/>
-      <c r="BU1" s="38"/>
-      <c r="BV1" s="40" t="s">
+      <c r="AZ1" s="41"/>
+      <c r="BA1" s="41"/>
+      <c r="BB1" s="41"/>
+      <c r="BC1" s="41"/>
+      <c r="BD1" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="BW1" s="39"/>
-      <c r="BX1" s="39"/>
-      <c r="BY1" s="39"/>
-      <c r="BZ1" s="40" t="s">
+      <c r="BE1" s="42"/>
+      <c r="BF1" s="42"/>
+      <c r="BG1" s="42"/>
+      <c r="BH1" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="CA1" s="40"/>
-      <c r="CB1" s="40"/>
-      <c r="CC1" s="40"/>
-      <c r="CD1" s="40"/>
-      <c r="CE1" s="38" t="s">
-        <v>15</v>
-      </c>
-      <c r="CF1" s="38"/>
-      <c r="CG1" s="38"/>
-      <c r="CH1" s="40" t="s">
+      <c r="BI1" s="41"/>
+      <c r="BJ1" s="41"/>
+      <c r="BK1" s="41"/>
+      <c r="BL1" s="41"/>
+      <c r="BM1" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="CI1" s="39"/>
-      <c r="CJ1" s="39"/>
-      <c r="CK1" s="39"/>
-      <c r="CL1" s="40" t="s">
+      <c r="BN1" s="42"/>
+      <c r="BO1" s="42"/>
+      <c r="BP1" s="42"/>
+      <c r="BQ1" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="CM1" s="40"/>
-      <c r="CN1" s="40"/>
-      <c r="CO1" s="40"/>
-      <c r="CP1" s="40"/>
-      <c r="CQ1" s="38" t="s">
-        <v>17</v>
-      </c>
-      <c r="CR1" s="38"/>
-      <c r="CS1" s="38"/>
-      <c r="CT1" s="40" t="s">
+      <c r="BR1" s="41"/>
+      <c r="BS1" s="41"/>
+      <c r="BT1" s="41"/>
+      <c r="BU1" s="41"/>
+      <c r="BV1" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="CU1" s="39"/>
-      <c r="CV1" s="39"/>
-      <c r="CW1" s="39"/>
-      <c r="CX1" s="40" t="s">
+      <c r="BW1" s="42"/>
+      <c r="BX1" s="42"/>
+      <c r="BY1" s="42"/>
+      <c r="BZ1" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="CY1" s="40"/>
-      <c r="CZ1" s="40"/>
-      <c r="DA1" s="40"/>
-      <c r="DB1" s="40"/>
-      <c r="DC1" s="38" t="s">
-        <v>19</v>
-      </c>
-      <c r="DD1" s="38"/>
-      <c r="DE1" s="38"/>
-    </row>
-    <row r="2" spans="1:109" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="CA1" s="41"/>
+      <c r="CB1" s="41"/>
+      <c r="CC1" s="41"/>
+      <c r="CD1" s="41"/>
+    </row>
+    <row r="2" spans="1:82" s="3" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>27</v>
       </c>
@@ -3173,308 +3126,227 @@
         <v>9</v>
       </c>
       <c r="K2" s="4">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="L2" s="5">
-        <v>11</v>
-      </c>
-      <c r="M2" s="6">
-        <v>12</v>
-      </c>
-      <c r="N2" s="4">
-        <v>13</v>
-      </c>
-      <c r="O2" s="5">
         <v>14</v>
       </c>
+      <c r="M2" s="5">
+        <v>15</v>
+      </c>
+      <c r="N2" s="6">
+        <v>16</v>
+      </c>
+      <c r="O2" s="4">
+        <v>17</v>
+      </c>
       <c r="P2" s="5">
-        <v>15</v>
-      </c>
-      <c r="Q2" s="6">
-        <v>16</v>
-      </c>
-      <c r="R2" s="4">
-        <v>17</v>
-      </c>
-      <c r="S2" s="5">
         <v>18</v>
       </c>
-      <c r="T2" s="5">
+      <c r="Q2" s="5">
         <v>19</v>
       </c>
+      <c r="R2" s="5">
+        <v>20</v>
+      </c>
+      <c r="S2" s="6">
+        <v>21</v>
+      </c>
+      <c r="T2" s="4">
+        <v>25</v>
+      </c>
       <c r="U2" s="5">
-        <v>20</v>
-      </c>
-      <c r="V2" s="6">
-        <v>21</v>
-      </c>
-      <c r="W2" s="4">
-        <v>22</v>
-      </c>
-      <c r="X2" s="5">
-        <v>23</v>
-      </c>
-      <c r="Y2" s="6">
-        <v>24</v>
-      </c>
-      <c r="Z2" s="4">
-        <v>25</v>
+        <v>26</v>
+      </c>
+      <c r="V2" s="5">
+        <v>27</v>
+      </c>
+      <c r="W2" s="6">
+        <v>28</v>
+      </c>
+      <c r="X2" s="4">
+        <v>29</v>
+      </c>
+      <c r="Y2" s="5">
+        <v>30</v>
+      </c>
+      <c r="Z2" s="5">
+        <v>31</v>
       </c>
       <c r="AA2" s="5">
-        <v>26</v>
-      </c>
-      <c r="AB2" s="5">
-        <v>27</v>
-      </c>
-      <c r="AC2" s="6">
-        <v>28</v>
-      </c>
-      <c r="AD2" s="4">
-        <v>29</v>
+        <v>32</v>
+      </c>
+      <c r="AB2" s="6">
+        <v>33</v>
+      </c>
+      <c r="AC2" s="4">
+        <v>37</v>
+      </c>
+      <c r="AD2" s="5">
+        <v>38</v>
       </c>
       <c r="AE2" s="5">
-        <v>30</v>
-      </c>
-      <c r="AF2" s="5">
-        <v>31</v>
-      </c>
-      <c r="AG2" s="5">
-        <v>32</v>
-      </c>
-      <c r="AH2" s="6">
-        <v>33</v>
-      </c>
-      <c r="AI2" s="4">
-        <v>34</v>
+        <v>39</v>
+      </c>
+      <c r="AF2" s="6">
+        <v>40</v>
+      </c>
+      <c r="AG2" s="4">
+        <v>41</v>
+      </c>
+      <c r="AH2" s="5">
+        <v>42</v>
+      </c>
+      <c r="AI2" s="5">
+        <v>43</v>
       </c>
       <c r="AJ2" s="5">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="AK2" s="6">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="AL2" s="4">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="AM2" s="5">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="AN2" s="5">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="AO2" s="6">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="AP2" s="4">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="AQ2" s="5">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="AR2" s="5">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="AS2" s="5">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="AT2" s="6">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="AU2" s="4">
-        <v>46</v>
+        <v>61</v>
       </c>
       <c r="AV2" s="5">
-        <v>47</v>
-      </c>
-      <c r="AW2" s="6">
-        <v>48</v>
-      </c>
-      <c r="AX2" s="4">
-        <v>49</v>
-      </c>
-      <c r="AY2" s="5">
-        <v>50</v>
+        <v>62</v>
+      </c>
+      <c r="AW2" s="5">
+        <v>63</v>
+      </c>
+      <c r="AX2" s="6">
+        <v>64</v>
+      </c>
+      <c r="AY2" s="4">
+        <v>65</v>
       </c>
       <c r="AZ2" s="5">
-        <v>51</v>
-      </c>
-      <c r="BA2" s="6">
-        <v>52</v>
-      </c>
-      <c r="BB2" s="4">
-        <v>53</v>
-      </c>
-      <c r="BC2" s="5">
-        <v>54</v>
-      </c>
-      <c r="BD2" s="5">
-        <v>55</v>
+        <v>66</v>
+      </c>
+      <c r="BA2" s="5">
+        <v>67</v>
+      </c>
+      <c r="BB2" s="5">
+        <v>68</v>
+      </c>
+      <c r="BC2" s="6">
+        <v>69</v>
+      </c>
+      <c r="BD2" s="4">
+        <v>73</v>
       </c>
       <c r="BE2" s="5">
-        <v>56</v>
-      </c>
-      <c r="BF2" s="6">
-        <v>57</v>
-      </c>
-      <c r="BG2" s="4">
-        <v>58</v>
-      </c>
-      <c r="BH2" s="5">
-        <v>59</v>
-      </c>
-      <c r="BI2" s="6">
-        <v>60</v>
-      </c>
-      <c r="BJ2" s="4">
-        <v>61</v>
+        <v>74</v>
+      </c>
+      <c r="BF2" s="5">
+        <v>75</v>
+      </c>
+      <c r="BG2" s="6">
+        <v>76</v>
+      </c>
+      <c r="BH2" s="4">
+        <v>77</v>
+      </c>
+      <c r="BI2" s="5">
+        <v>78</v>
+      </c>
+      <c r="BJ2" s="5">
+        <v>79</v>
       </c>
       <c r="BK2" s="5">
-        <v>62</v>
-      </c>
-      <c r="BL2" s="5">
-        <v>63</v>
-      </c>
-      <c r="BM2" s="6">
-        <v>64</v>
-      </c>
-      <c r="BN2" s="4">
-        <v>65</v>
+        <v>80</v>
+      </c>
+      <c r="BL2" s="6">
+        <v>81</v>
+      </c>
+      <c r="BM2" s="4">
+        <v>85</v>
+      </c>
+      <c r="BN2" s="5">
+        <v>86</v>
       </c>
       <c r="BO2" s="5">
-        <v>66</v>
-      </c>
-      <c r="BP2" s="5">
-        <v>67</v>
-      </c>
-      <c r="BQ2" s="5">
-        <v>68</v>
-      </c>
-      <c r="BR2" s="6">
-        <v>69</v>
-      </c>
-      <c r="BS2" s="4">
-        <v>70</v>
+        <v>87</v>
+      </c>
+      <c r="BP2" s="6">
+        <v>88</v>
+      </c>
+      <c r="BQ2" s="4">
+        <v>89</v>
+      </c>
+      <c r="BR2" s="5">
+        <v>90</v>
+      </c>
+      <c r="BS2" s="5">
+        <v>91</v>
       </c>
       <c r="BT2" s="5">
-        <v>71</v>
+        <v>92</v>
       </c>
       <c r="BU2" s="6">
-        <v>72</v>
+        <v>93</v>
       </c>
       <c r="BV2" s="4">
-        <v>73</v>
+        <v>97</v>
       </c>
       <c r="BW2" s="5">
-        <v>74</v>
+        <v>98</v>
       </c>
       <c r="BX2" s="5">
-        <v>75</v>
+        <v>99</v>
       </c>
       <c r="BY2" s="6">
-        <v>76</v>
+        <v>100</v>
       </c>
       <c r="BZ2" s="4">
-        <v>77</v>
+        <v>101</v>
       </c>
       <c r="CA2" s="5">
-        <v>78</v>
+        <v>102</v>
       </c>
       <c r="CB2" s="5">
-        <v>79</v>
+        <v>103</v>
       </c>
       <c r="CC2" s="5">
-        <v>80</v>
+        <v>104</v>
       </c>
       <c r="CD2" s="6">
-        <v>81</v>
-      </c>
-      <c r="CE2" s="4">
-        <v>82</v>
-      </c>
-      <c r="CF2" s="5">
-        <v>83</v>
-      </c>
-      <c r="CG2" s="6">
-        <v>84</v>
-      </c>
-      <c r="CH2" s="4">
-        <v>85</v>
-      </c>
-      <c r="CI2" s="5">
-        <v>86</v>
-      </c>
-      <c r="CJ2" s="5">
-        <v>87</v>
-      </c>
-      <c r="CK2" s="6">
-        <v>88</v>
-      </c>
-      <c r="CL2" s="4">
-        <v>89</v>
-      </c>
-      <c r="CM2" s="5">
-        <v>90</v>
-      </c>
-      <c r="CN2" s="5">
-        <v>91</v>
-      </c>
-      <c r="CO2" s="5">
-        <v>92</v>
-      </c>
-      <c r="CP2" s="6">
-        <v>93</v>
-      </c>
-      <c r="CQ2" s="4">
-        <v>94</v>
-      </c>
-      <c r="CR2" s="5">
-        <v>95</v>
-      </c>
-      <c r="CS2" s="6">
-        <v>96</v>
-      </c>
-      <c r="CT2" s="4">
-        <v>97</v>
-      </c>
-      <c r="CU2" s="5">
-        <v>98</v>
-      </c>
-      <c r="CV2" s="5">
-        <v>99</v>
-      </c>
-      <c r="CW2" s="6">
-        <v>100</v>
-      </c>
-      <c r="CX2" s="4">
-        <v>101</v>
-      </c>
-      <c r="CY2" s="5">
-        <v>102</v>
-      </c>
-      <c r="CZ2" s="5">
-        <v>103</v>
-      </c>
-      <c r="DA2" s="5">
-        <v>104</v>
-      </c>
-      <c r="DB2" s="6">
         <v>105</v>
       </c>
-      <c r="DC2" s="4">
-        <v>106</v>
-      </c>
-      <c r="DD2" s="5">
-        <v>107</v>
-      </c>
-      <c r="DE2" s="6">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="3" spans="1:109" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:82" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="41"/>
+      <c r="B3" s="30"/>
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
       <c r="E3" s="10"/>
@@ -3554,40 +3426,13 @@
       <c r="CA3" s="10"/>
       <c r="CB3" s="10"/>
       <c r="CC3" s="10"/>
-      <c r="CD3" s="10"/>
-      <c r="CE3" s="10"/>
-      <c r="CF3" s="10"/>
-      <c r="CG3" s="10"/>
-      <c r="CH3" s="10"/>
-      <c r="CI3" s="10"/>
-      <c r="CJ3" s="10"/>
-      <c r="CK3" s="10"/>
-      <c r="CL3" s="10"/>
-      <c r="CM3" s="10"/>
-      <c r="CN3" s="10"/>
-      <c r="CO3" s="10"/>
-      <c r="CP3" s="10"/>
-      <c r="CQ3" s="10"/>
-      <c r="CR3" s="10"/>
-      <c r="CS3" s="10"/>
-      <c r="CT3" s="10"/>
-      <c r="CU3" s="10"/>
-      <c r="CV3" s="10"/>
-      <c r="CW3" s="10"/>
-      <c r="CX3" s="10"/>
-      <c r="CY3" s="10"/>
-      <c r="CZ3" s="10"/>
-      <c r="DA3" s="10"/>
-      <c r="DB3" s="10"/>
-      <c r="DC3" s="10"/>
-      <c r="DD3" s="10"/>
-      <c r="DE3" s="11"/>
-    </row>
-    <row r="4" spans="1:109" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="CD3" s="11"/>
+    </row>
+    <row r="4" spans="1:82" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" s="42"/>
+        <v>39</v>
+      </c>
+      <c r="B4" s="31"/>
       <c r="C4" s="14"/>
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
@@ -3667,41 +3512,14 @@
       <c r="CA4" s="12"/>
       <c r="CB4" s="12"/>
       <c r="CC4" s="12"/>
-      <c r="CD4" s="12"/>
-      <c r="CE4" s="12"/>
-      <c r="CF4" s="12"/>
-      <c r="CG4" s="12"/>
-      <c r="CH4" s="12"/>
-      <c r="CI4" s="12"/>
-      <c r="CJ4" s="12"/>
-      <c r="CK4" s="12"/>
-      <c r="CL4" s="12"/>
-      <c r="CM4" s="12"/>
-      <c r="CN4" s="12"/>
-      <c r="CO4" s="12"/>
-      <c r="CP4" s="12"/>
-      <c r="CQ4" s="12"/>
-      <c r="CR4" s="12"/>
-      <c r="CS4" s="12"/>
-      <c r="CT4" s="12"/>
-      <c r="CU4" s="12"/>
-      <c r="CV4" s="12"/>
-      <c r="CW4" s="12"/>
-      <c r="CX4" s="12"/>
-      <c r="CY4" s="12"/>
-      <c r="CZ4" s="12"/>
-      <c r="DA4" s="12"/>
-      <c r="DB4" s="12"/>
-      <c r="DC4" s="12"/>
-      <c r="DD4" s="12"/>
-      <c r="DE4" s="13"/>
-    </row>
-    <row r="5" spans="1:109" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="CD4" s="13"/>
+    </row>
+    <row r="5" spans="1:82" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>31</v>
       </c>
       <c r="B5" s="22"/>
-      <c r="C5" s="43"/>
+      <c r="C5" s="32"/>
       <c r="D5" s="14"/>
       <c r="E5" s="14"/>
       <c r="F5" s="14"/>
@@ -3780,50 +3598,23 @@
       <c r="CA5" s="12"/>
       <c r="CB5" s="12"/>
       <c r="CC5" s="12"/>
-      <c r="CD5" s="12"/>
-      <c r="CE5" s="12"/>
-      <c r="CF5" s="12"/>
-      <c r="CG5" s="12"/>
-      <c r="CH5" s="12"/>
-      <c r="CI5" s="12"/>
-      <c r="CJ5" s="12"/>
-      <c r="CK5" s="12"/>
-      <c r="CL5" s="12"/>
-      <c r="CM5" s="12"/>
-      <c r="CN5" s="12"/>
-      <c r="CO5" s="12"/>
-      <c r="CP5" s="12"/>
-      <c r="CQ5" s="12"/>
-      <c r="CR5" s="12"/>
-      <c r="CS5" s="12"/>
-      <c r="CT5" s="12"/>
-      <c r="CU5" s="12"/>
-      <c r="CV5" s="12"/>
-      <c r="CW5" s="12"/>
-      <c r="CX5" s="12"/>
-      <c r="CY5" s="12"/>
-      <c r="CZ5" s="12"/>
-      <c r="DA5" s="12"/>
-      <c r="DB5" s="12"/>
-      <c r="DC5" s="12"/>
-      <c r="DD5" s="12"/>
-      <c r="DE5" s="13"/>
-    </row>
-    <row r="6" spans="1:109" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="CD5" s="13"/>
+    </row>
+    <row r="6" spans="1:82" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>32</v>
       </c>
       <c r="B6" s="22"/>
       <c r="C6" s="12"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
       <c r="F6" s="12"/>
       <c r="G6" s="14"/>
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>
       <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
       <c r="M6" s="12"/>
       <c r="N6" s="12"/>
       <c r="O6" s="12"/>
@@ -3893,36 +3684,9 @@
       <c r="CA6" s="12"/>
       <c r="CB6" s="12"/>
       <c r="CC6" s="12"/>
-      <c r="CD6" s="12"/>
-      <c r="CE6" s="12"/>
-      <c r="CF6" s="12"/>
-      <c r="CG6" s="12"/>
-      <c r="CH6" s="12"/>
-      <c r="CI6" s="12"/>
-      <c r="CJ6" s="12"/>
-      <c r="CK6" s="12"/>
-      <c r="CL6" s="12"/>
-      <c r="CM6" s="12"/>
-      <c r="CN6" s="12"/>
-      <c r="CO6" s="12"/>
-      <c r="CP6" s="12"/>
-      <c r="CQ6" s="12"/>
-      <c r="CR6" s="12"/>
-      <c r="CS6" s="12"/>
-      <c r="CT6" s="12"/>
-      <c r="CU6" s="12"/>
-      <c r="CV6" s="12"/>
-      <c r="CW6" s="12"/>
-      <c r="CX6" s="12"/>
-      <c r="CY6" s="12"/>
-      <c r="CZ6" s="12"/>
-      <c r="DA6" s="12"/>
-      <c r="DB6" s="12"/>
-      <c r="DC6" s="12"/>
-      <c r="DD6" s="12"/>
-      <c r="DE6" s="13"/>
-    </row>
-    <row r="7" spans="1:109" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="CD6" s="13"/>
+    </row>
+    <row r="7" spans="1:82" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>35</v>
       </c>
@@ -3935,14 +3699,14 @@
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
       <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
       <c r="M7" s="14"/>
-      <c r="N7" s="14"/>
-      <c r="O7" s="14"/>
-      <c r="P7" s="14"/>
-      <c r="Q7" s="12"/>
-      <c r="R7" s="12"/>
+      <c r="N7" s="32"/>
+      <c r="O7" s="32"/>
+      <c r="P7" s="32"/>
+      <c r="Q7" s="32"/>
+      <c r="R7" s="32"/>
       <c r="S7" s="12"/>
       <c r="T7" s="12"/>
       <c r="U7" s="12"/>
@@ -4006,36 +3770,9 @@
       <c r="CA7" s="12"/>
       <c r="CB7" s="12"/>
       <c r="CC7" s="12"/>
-      <c r="CD7" s="12"/>
-      <c r="CE7" s="12"/>
-      <c r="CF7" s="12"/>
-      <c r="CG7" s="12"/>
-      <c r="CH7" s="12"/>
-      <c r="CI7" s="12"/>
-      <c r="CJ7" s="12"/>
-      <c r="CK7" s="12"/>
-      <c r="CL7" s="12"/>
-      <c r="CM7" s="12"/>
-      <c r="CN7" s="12"/>
-      <c r="CO7" s="12"/>
-      <c r="CP7" s="12"/>
-      <c r="CQ7" s="12"/>
-      <c r="CR7" s="12"/>
-      <c r="CS7" s="12"/>
-      <c r="CT7" s="12"/>
-      <c r="CU7" s="12"/>
-      <c r="CV7" s="12"/>
-      <c r="CW7" s="12"/>
-      <c r="CX7" s="12"/>
-      <c r="CY7" s="12"/>
-      <c r="CZ7" s="12"/>
-      <c r="DA7" s="12"/>
-      <c r="DB7" s="12"/>
-      <c r="DC7" s="12"/>
-      <c r="DD7" s="12"/>
-      <c r="DE7" s="13"/>
-    </row>
-    <row r="8" spans="1:109" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="CD7" s="13"/>
+    </row>
+    <row r="8" spans="1:82" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>37</v>
       </c>
@@ -4054,11 +3791,11 @@
       <c r="N8" s="12"/>
       <c r="O8" s="12"/>
       <c r="P8" s="12"/>
-      <c r="Q8" s="14"/>
-      <c r="R8" s="14"/>
+      <c r="Q8" s="12"/>
+      <c r="R8" s="12"/>
       <c r="S8" s="14"/>
-      <c r="T8" s="14"/>
-      <c r="U8" s="14"/>
+      <c r="T8" s="12"/>
+      <c r="U8" s="12"/>
       <c r="V8" s="12"/>
       <c r="W8" s="12"/>
       <c r="X8" s="12"/>
@@ -4084,15 +3821,15 @@
       <c r="AR8" s="12"/>
       <c r="AS8" s="12"/>
       <c r="AT8" s="12"/>
-      <c r="AU8" s="12"/>
-      <c r="AV8" s="12"/>
-      <c r="AW8" s="12"/>
-      <c r="AX8" s="12"/>
-      <c r="AY8" s="12"/>
-      <c r="AZ8" s="12"/>
-      <c r="BA8" s="12"/>
-      <c r="BB8" s="12"/>
-      <c r="BC8" s="12"/>
+      <c r="AU8" s="32"/>
+      <c r="AV8" s="32"/>
+      <c r="AW8" s="32"/>
+      <c r="AX8" s="32"/>
+      <c r="AY8" s="32"/>
+      <c r="AZ8" s="32"/>
+      <c r="BA8" s="32"/>
+      <c r="BB8" s="27"/>
+      <c r="BC8" s="27"/>
       <c r="BD8" s="12"/>
       <c r="BE8" s="12"/>
       <c r="BF8" s="12"/>
@@ -4119,38 +3856,11 @@
       <c r="CA8" s="12"/>
       <c r="CB8" s="12"/>
       <c r="CC8" s="12"/>
-      <c r="CD8" s="12"/>
-      <c r="CE8" s="12"/>
-      <c r="CF8" s="12"/>
-      <c r="CG8" s="12"/>
-      <c r="CH8" s="12"/>
-      <c r="CI8" s="12"/>
-      <c r="CJ8" s="12"/>
-      <c r="CK8" s="12"/>
-      <c r="CL8" s="12"/>
-      <c r="CM8" s="12"/>
-      <c r="CN8" s="12"/>
-      <c r="CO8" s="12"/>
-      <c r="CP8" s="12"/>
-      <c r="CQ8" s="12"/>
-      <c r="CR8" s="12"/>
-      <c r="CS8" s="12"/>
-      <c r="CT8" s="12"/>
-      <c r="CU8" s="12"/>
-      <c r="CV8" s="12"/>
-      <c r="CW8" s="12"/>
-      <c r="CX8" s="12"/>
-      <c r="CY8" s="12"/>
-      <c r="CZ8" s="12"/>
-      <c r="DA8" s="12"/>
-      <c r="DB8" s="12"/>
-      <c r="DC8" s="12"/>
-      <c r="DD8" s="12"/>
-      <c r="DE8" s="13"/>
-    </row>
-    <row r="9" spans="1:109" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="CD8" s="13"/>
+    </row>
+    <row r="9" spans="1:82" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B9" s="22"/>
       <c r="C9" s="12"/>
@@ -4170,16 +3880,16 @@
       <c r="Q9" s="12"/>
       <c r="R9" s="12"/>
       <c r="S9" s="12"/>
-      <c r="T9" s="12"/>
-      <c r="U9" s="12"/>
-      <c r="V9" s="14"/>
-      <c r="W9" s="14"/>
-      <c r="X9" s="14"/>
+      <c r="T9" s="14"/>
+      <c r="U9" s="14"/>
+      <c r="V9" s="12"/>
+      <c r="W9" s="12"/>
+      <c r="X9" s="12"/>
       <c r="Y9" s="12"/>
       <c r="Z9" s="12"/>
       <c r="AA9" s="12"/>
       <c r="AB9" s="12"/>
-      <c r="AC9" s="12"/>
+      <c r="AC9" s="43"/>
       <c r="AD9" s="12"/>
       <c r="AE9" s="12"/>
       <c r="AF9" s="12"/>
@@ -4204,8 +3914,8 @@
       <c r="AY9" s="12"/>
       <c r="AZ9" s="12"/>
       <c r="BA9" s="12"/>
-      <c r="BB9" s="12"/>
-      <c r="BC9" s="12"/>
+      <c r="BB9" s="32"/>
+      <c r="BC9" s="32"/>
       <c r="BD9" s="12"/>
       <c r="BE9" s="12"/>
       <c r="BF9" s="12"/>
@@ -4232,38 +3942,11 @@
       <c r="CA9" s="12"/>
       <c r="CB9" s="12"/>
       <c r="CC9" s="12"/>
-      <c r="CD9" s="12"/>
-      <c r="CE9" s="12"/>
-      <c r="CF9" s="12"/>
-      <c r="CG9" s="12"/>
-      <c r="CH9" s="12"/>
-      <c r="CI9" s="12"/>
-      <c r="CJ9" s="12"/>
-      <c r="CK9" s="12"/>
-      <c r="CL9" s="12"/>
-      <c r="CM9" s="12"/>
-      <c r="CN9" s="12"/>
-      <c r="CO9" s="12"/>
-      <c r="CP9" s="12"/>
-      <c r="CQ9" s="12"/>
-      <c r="CR9" s="12"/>
-      <c r="CS9" s="12"/>
-      <c r="CT9" s="12"/>
-      <c r="CU9" s="12"/>
-      <c r="CV9" s="12"/>
-      <c r="CW9" s="12"/>
-      <c r="CX9" s="12"/>
-      <c r="CY9" s="12"/>
-      <c r="CZ9" s="12"/>
-      <c r="DA9" s="12"/>
-      <c r="DB9" s="12"/>
-      <c r="DC9" s="12"/>
-      <c r="DD9" s="12"/>
-      <c r="DE9" s="13"/>
-    </row>
-    <row r="10" spans="1:109" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="CD9" s="13"/>
+    </row>
+    <row r="10" spans="1:82" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B10" s="22"/>
       <c r="C10" s="12"/>
@@ -4282,15 +3965,15 @@
       <c r="P10" s="12"/>
       <c r="Q10" s="12"/>
       <c r="R10" s="12"/>
-      <c r="S10" s="12"/>
-      <c r="T10" s="12"/>
-      <c r="U10" s="12"/>
-      <c r="V10" s="12"/>
-      <c r="W10" s="12"/>
-      <c r="X10" s="12"/>
+      <c r="S10" s="32"/>
+      <c r="T10" s="32"/>
+      <c r="U10" s="32"/>
+      <c r="V10" s="32"/>
+      <c r="W10" s="14"/>
+      <c r="X10" s="14"/>
       <c r="Y10" s="14"/>
       <c r="Z10" s="14"/>
-      <c r="AA10" s="14"/>
+      <c r="AA10" s="12"/>
       <c r="AB10" s="12"/>
       <c r="AC10" s="12"/>
       <c r="AD10" s="12"/>
@@ -4301,7 +3984,7 @@
       <c r="AI10" s="12"/>
       <c r="AJ10" s="12"/>
       <c r="AK10" s="12"/>
-      <c r="AL10" s="43"/>
+      <c r="AL10" s="12"/>
       <c r="AM10" s="12"/>
       <c r="AN10" s="12"/>
       <c r="AO10" s="12"/>
@@ -4345,38 +4028,11 @@
       <c r="CA10" s="12"/>
       <c r="CB10" s="12"/>
       <c r="CC10" s="12"/>
-      <c r="CD10" s="12"/>
-      <c r="CE10" s="12"/>
-      <c r="CF10" s="12"/>
-      <c r="CG10" s="12"/>
-      <c r="CH10" s="12"/>
-      <c r="CI10" s="12"/>
-      <c r="CJ10" s="12"/>
-      <c r="CK10" s="12"/>
-      <c r="CL10" s="12"/>
-      <c r="CM10" s="12"/>
-      <c r="CN10" s="12"/>
-      <c r="CO10" s="12"/>
-      <c r="CP10" s="12"/>
-      <c r="CQ10" s="12"/>
-      <c r="CR10" s="12"/>
-      <c r="CS10" s="12"/>
-      <c r="CT10" s="12"/>
-      <c r="CU10" s="12"/>
-      <c r="CV10" s="12"/>
-      <c r="CW10" s="12"/>
-      <c r="CX10" s="12"/>
-      <c r="CY10" s="12"/>
-      <c r="CZ10" s="12"/>
-      <c r="DA10" s="12"/>
-      <c r="DB10" s="12"/>
-      <c r="DC10" s="12"/>
-      <c r="DD10" s="12"/>
-      <c r="DE10" s="13"/>
-    </row>
-    <row r="11" spans="1:109" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="CD10" s="13"/>
+    </row>
+    <row r="11" spans="1:82" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B11" s="22"/>
       <c r="C11" s="12"/>
@@ -4399,24 +4055,24 @@
       <c r="T11" s="12"/>
       <c r="U11" s="12"/>
       <c r="V11" s="12"/>
-      <c r="W11" s="12"/>
-      <c r="X11" s="12"/>
-      <c r="Y11" s="43"/>
-      <c r="Z11" s="43"/>
-      <c r="AA11" s="43"/>
-      <c r="AB11" s="43"/>
-      <c r="AC11" s="14"/>
-      <c r="AD11" s="14"/>
-      <c r="AE11" s="14"/>
-      <c r="AF11" s="14"/>
-      <c r="AG11" s="12"/>
-      <c r="AH11" s="12"/>
-      <c r="AI11" s="12"/>
-      <c r="AJ11" s="12"/>
-      <c r="AK11" s="12"/>
-      <c r="AL11" s="12"/>
-      <c r="AM11" s="12"/>
-      <c r="AN11" s="12"/>
+      <c r="W11" s="32"/>
+      <c r="X11" s="32"/>
+      <c r="Y11" s="32"/>
+      <c r="Z11" s="32"/>
+      <c r="AA11" s="32"/>
+      <c r="AB11" s="32"/>
+      <c r="AC11" s="32"/>
+      <c r="AD11" s="32"/>
+      <c r="AE11" s="32"/>
+      <c r="AF11" s="32"/>
+      <c r="AG11" s="32"/>
+      <c r="AH11" s="32"/>
+      <c r="AI11" s="32"/>
+      <c r="AJ11" s="32"/>
+      <c r="AK11" s="32"/>
+      <c r="AL11" s="32"/>
+      <c r="AM11" s="32"/>
+      <c r="AN11" s="32"/>
       <c r="AO11" s="12"/>
       <c r="AP11" s="12"/>
       <c r="AQ11" s="12"/>
@@ -4458,38 +4114,11 @@
       <c r="CA11" s="12"/>
       <c r="CB11" s="12"/>
       <c r="CC11" s="12"/>
-      <c r="CD11" s="12"/>
-      <c r="CE11" s="12"/>
-      <c r="CF11" s="12"/>
-      <c r="CG11" s="12"/>
-      <c r="CH11" s="12"/>
-      <c r="CI11" s="12"/>
-      <c r="CJ11" s="12"/>
-      <c r="CK11" s="12"/>
-      <c r="CL11" s="12"/>
-      <c r="CM11" s="12"/>
-      <c r="CN11" s="12"/>
-      <c r="CO11" s="12"/>
-      <c r="CP11" s="12"/>
-      <c r="CQ11" s="12"/>
-      <c r="CR11" s="12"/>
-      <c r="CS11" s="12"/>
-      <c r="CT11" s="12"/>
-      <c r="CU11" s="12"/>
-      <c r="CV11" s="12"/>
-      <c r="CW11" s="12"/>
-      <c r="CX11" s="12"/>
-      <c r="CY11" s="12"/>
-      <c r="CZ11" s="12"/>
-      <c r="DA11" s="12"/>
-      <c r="DB11" s="12"/>
-      <c r="DC11" s="12"/>
-      <c r="DD11" s="12"/>
-      <c r="DE11" s="13"/>
-    </row>
-    <row r="12" spans="1:109" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="CD11" s="13"/>
+    </row>
+    <row r="12" spans="1:82" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B12" s="22"/>
       <c r="C12" s="12"/>
@@ -4518,24 +4147,24 @@
       <c r="Z12" s="12"/>
       <c r="AA12" s="12"/>
       <c r="AB12" s="12"/>
-      <c r="AC12" s="43"/>
-      <c r="AD12" s="43"/>
-      <c r="AE12" s="43"/>
-      <c r="AF12" s="43"/>
-      <c r="AG12" s="43"/>
-      <c r="AH12" s="43"/>
-      <c r="AI12" s="43"/>
-      <c r="AJ12" s="43"/>
-      <c r="AK12" s="43"/>
-      <c r="AL12" s="43"/>
-      <c r="AM12" s="43"/>
-      <c r="AN12" s="43"/>
-      <c r="AO12" s="43"/>
-      <c r="AP12" s="43"/>
-      <c r="AQ12" s="43"/>
-      <c r="AR12" s="43"/>
-      <c r="AS12" s="43"/>
-      <c r="AT12" s="43"/>
+      <c r="AC12" s="12"/>
+      <c r="AD12" s="32"/>
+      <c r="AE12" s="14"/>
+      <c r="AF12" s="14"/>
+      <c r="AG12" s="14"/>
+      <c r="AH12" s="12"/>
+      <c r="AI12" s="12"/>
+      <c r="AJ12" s="12"/>
+      <c r="AK12" s="12"/>
+      <c r="AL12" s="12"/>
+      <c r="AM12" s="12"/>
+      <c r="AN12" s="12"/>
+      <c r="AO12" s="12"/>
+      <c r="AP12" s="12"/>
+      <c r="AQ12" s="12"/>
+      <c r="AR12" s="12"/>
+      <c r="AS12" s="12"/>
+      <c r="AT12" s="12"/>
       <c r="AU12" s="12"/>
       <c r="AV12" s="12"/>
       <c r="AW12" s="12"/>
@@ -4571,38 +4200,11 @@
       <c r="CA12" s="12"/>
       <c r="CB12" s="12"/>
       <c r="CC12" s="12"/>
-      <c r="CD12" s="12"/>
-      <c r="CE12" s="12"/>
-      <c r="CF12" s="12"/>
-      <c r="CG12" s="12"/>
-      <c r="CH12" s="12"/>
-      <c r="CI12" s="12"/>
-      <c r="CJ12" s="12"/>
-      <c r="CK12" s="12"/>
-      <c r="CL12" s="12"/>
-      <c r="CM12" s="12"/>
-      <c r="CN12" s="12"/>
-      <c r="CO12" s="12"/>
-      <c r="CP12" s="12"/>
-      <c r="CQ12" s="12"/>
-      <c r="CR12" s="12"/>
-      <c r="CS12" s="12"/>
-      <c r="CT12" s="12"/>
-      <c r="CU12" s="12"/>
-      <c r="CV12" s="12"/>
-      <c r="CW12" s="12"/>
-      <c r="CX12" s="12"/>
-      <c r="CY12" s="12"/>
-      <c r="CZ12" s="12"/>
-      <c r="DA12" s="12"/>
-      <c r="DB12" s="12"/>
-      <c r="DC12" s="12"/>
-      <c r="DD12" s="12"/>
-      <c r="DE12" s="13"/>
-    </row>
-    <row r="13" spans="1:109" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="CD12" s="13"/>
+    </row>
+    <row r="13" spans="1:82" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="B13" s="22"/>
       <c r="C13" s="12"/>
@@ -4610,8 +4212,8 @@
       <c r="E13" s="12"/>
       <c r="F13" s="12"/>
       <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
+      <c r="H13" s="32"/>
+      <c r="I13" s="32"/>
       <c r="J13" s="12"/>
       <c r="K13" s="12"/>
       <c r="L13" s="12"/>
@@ -4636,11 +4238,11 @@
       <c r="AE13" s="12"/>
       <c r="AF13" s="12"/>
       <c r="AG13" s="12"/>
-      <c r="AH13" s="12"/>
-      <c r="AI13" s="12"/>
-      <c r="AJ13" s="12"/>
-      <c r="AK13" s="43"/>
-      <c r="AL13" s="12"/>
+      <c r="AH13" s="14"/>
+      <c r="AI13" s="14"/>
+      <c r="AJ13" s="14"/>
+      <c r="AK13" s="14"/>
+      <c r="AL13" s="14"/>
       <c r="AM13" s="14"/>
       <c r="AN13" s="14"/>
       <c r="AO13" s="14"/>
@@ -4684,36 +4286,9 @@
       <c r="CA13" s="12"/>
       <c r="CB13" s="12"/>
       <c r="CC13" s="12"/>
-      <c r="CD13" s="12"/>
-      <c r="CE13" s="12"/>
-      <c r="CF13" s="12"/>
-      <c r="CG13" s="12"/>
-      <c r="CH13" s="12"/>
-      <c r="CI13" s="12"/>
-      <c r="CJ13" s="12"/>
-      <c r="CK13" s="12"/>
-      <c r="CL13" s="12"/>
-      <c r="CM13" s="12"/>
-      <c r="CN13" s="12"/>
-      <c r="CO13" s="12"/>
-      <c r="CP13" s="12"/>
-      <c r="CQ13" s="12"/>
-      <c r="CR13" s="12"/>
-      <c r="CS13" s="12"/>
-      <c r="CT13" s="12"/>
-      <c r="CU13" s="12"/>
-      <c r="CV13" s="12"/>
-      <c r="CW13" s="12"/>
-      <c r="CX13" s="12"/>
-      <c r="CY13" s="12"/>
-      <c r="CZ13" s="12"/>
-      <c r="DA13" s="12"/>
-      <c r="DB13" s="12"/>
-      <c r="DC13" s="12"/>
-      <c r="DD13" s="12"/>
-      <c r="DE13" s="13"/>
-    </row>
-    <row r="14" spans="1:109" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="CD13" s="13"/>
+    </row>
+    <row r="14" spans="1:82" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>41</v>
       </c>
@@ -4723,12 +4298,12 @@
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
-      <c r="H14" s="43"/>
-      <c r="I14" s="43"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="43"/>
+      <c r="K14" s="43"/>
+      <c r="L14" s="43"/>
+      <c r="M14" s="43"/>
       <c r="N14" s="12"/>
       <c r="O14" s="12"/>
       <c r="P14" s="12"/>
@@ -4753,23 +4328,23 @@
       <c r="AI14" s="12"/>
       <c r="AJ14" s="12"/>
       <c r="AK14" s="12"/>
-      <c r="AL14" s="12"/>
-      <c r="AM14" s="12"/>
-      <c r="AN14" s="12"/>
-      <c r="AO14" s="12"/>
-      <c r="AP14" s="12"/>
-      <c r="AQ14" s="14"/>
-      <c r="AR14" s="14"/>
-      <c r="AS14" s="14"/>
-      <c r="AT14" s="14"/>
-      <c r="AU14" s="14"/>
-      <c r="AV14" s="14"/>
-      <c r="AW14" s="14"/>
-      <c r="AX14" s="14"/>
-      <c r="AY14" s="14"/>
-      <c r="AZ14" s="14"/>
-      <c r="BA14" s="14"/>
-      <c r="BB14" s="14"/>
+      <c r="AL14" s="32"/>
+      <c r="AM14" s="32"/>
+      <c r="AN14" s="32"/>
+      <c r="AO14" s="32"/>
+      <c r="AP14" s="32"/>
+      <c r="AQ14" s="32"/>
+      <c r="AR14" s="32"/>
+      <c r="AS14" s="32"/>
+      <c r="AT14" s="32"/>
+      <c r="AU14" s="12"/>
+      <c r="AV14" s="12"/>
+      <c r="AW14" s="12"/>
+      <c r="AX14" s="12"/>
+      <c r="AY14" s="12"/>
+      <c r="AZ14" s="12"/>
+      <c r="BA14" s="12"/>
+      <c r="BB14" s="12"/>
       <c r="BC14" s="12"/>
       <c r="BD14" s="12"/>
       <c r="BE14" s="12"/>
@@ -4797,36 +4372,9 @@
       <c r="CA14" s="12"/>
       <c r="CB14" s="12"/>
       <c r="CC14" s="12"/>
-      <c r="CD14" s="12"/>
-      <c r="CE14" s="12"/>
-      <c r="CF14" s="12"/>
-      <c r="CG14" s="12"/>
-      <c r="CH14" s="12"/>
-      <c r="CI14" s="12"/>
-      <c r="CJ14" s="12"/>
-      <c r="CK14" s="12"/>
-      <c r="CL14" s="12"/>
-      <c r="CM14" s="12"/>
-      <c r="CN14" s="12"/>
-      <c r="CO14" s="12"/>
-      <c r="CP14" s="12"/>
-      <c r="CQ14" s="12"/>
-      <c r="CR14" s="12"/>
-      <c r="CS14" s="12"/>
-      <c r="CT14" s="12"/>
-      <c r="CU14" s="12"/>
-      <c r="CV14" s="12"/>
-      <c r="CW14" s="12"/>
-      <c r="CX14" s="12"/>
-      <c r="CY14" s="12"/>
-      <c r="CZ14" s="12"/>
-      <c r="DA14" s="12"/>
-      <c r="DB14" s="12"/>
-      <c r="DC14" s="12"/>
-      <c r="DD14" s="12"/>
-      <c r="DE14" s="13"/>
-    </row>
-    <row r="15" spans="1:109" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="CD14" s="13"/>
+    </row>
+    <row r="15" spans="1:82" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>42</v>
       </c>
@@ -4838,8 +4386,8 @@
       <c r="G15" s="12"/>
       <c r="H15" s="12"/>
       <c r="I15" s="12"/>
-      <c r="J15" s="43"/>
-      <c r="K15" s="43"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
       <c r="L15" s="12"/>
       <c r="M15" s="12"/>
       <c r="N15" s="12"/>
@@ -4880,24 +4428,24 @@
       <c r="AW15" s="12"/>
       <c r="AX15" s="12"/>
       <c r="AY15" s="12"/>
-      <c r="AZ15" s="12"/>
-      <c r="BA15" s="12"/>
-      <c r="BB15" s="12"/>
+      <c r="AZ15" s="14"/>
+      <c r="BA15" s="14"/>
+      <c r="BB15" s="14"/>
       <c r="BC15" s="14"/>
       <c r="BD15" s="14"/>
       <c r="BE15" s="14"/>
       <c r="BF15" s="14"/>
       <c r="BG15" s="14"/>
       <c r="BH15" s="14"/>
-      <c r="BI15" s="12"/>
-      <c r="BJ15" s="12"/>
-      <c r="BK15" s="12"/>
-      <c r="BL15" s="12"/>
-      <c r="BM15" s="12"/>
-      <c r="BN15" s="12"/>
-      <c r="BO15" s="12"/>
-      <c r="BP15" s="12"/>
-      <c r="BQ15" s="12"/>
+      <c r="BI15" s="14"/>
+      <c r="BJ15" s="14"/>
+      <c r="BK15" s="14"/>
+      <c r="BL15" s="14"/>
+      <c r="BM15" s="14"/>
+      <c r="BN15" s="14"/>
+      <c r="BO15" s="14"/>
+      <c r="BP15" s="14"/>
+      <c r="BQ15" s="27"/>
       <c r="BR15" s="12"/>
       <c r="BS15" s="12"/>
       <c r="BT15" s="12"/>
@@ -4910,416 +4458,127 @@
       <c r="CA15" s="12"/>
       <c r="CB15" s="12"/>
       <c r="CC15" s="12"/>
-      <c r="CD15" s="12"/>
-      <c r="CE15" s="12"/>
-      <c r="CF15" s="12"/>
-      <c r="CG15" s="12"/>
-      <c r="CH15" s="12"/>
-      <c r="CI15" s="12"/>
-      <c r="CJ15" s="12"/>
-      <c r="CK15" s="12"/>
-      <c r="CL15" s="12"/>
-      <c r="CM15" s="12"/>
-      <c r="CN15" s="12"/>
-      <c r="CO15" s="12"/>
-      <c r="CP15" s="12"/>
-      <c r="CQ15" s="12"/>
-      <c r="CR15" s="12"/>
-      <c r="CS15" s="12"/>
-      <c r="CT15" s="12"/>
-      <c r="CU15" s="12"/>
-      <c r="CV15" s="12"/>
-      <c r="CW15" s="12"/>
-      <c r="CX15" s="12"/>
-      <c r="CY15" s="12"/>
-      <c r="CZ15" s="12"/>
-      <c r="DA15" s="12"/>
-      <c r="DB15" s="12"/>
-      <c r="DC15" s="12"/>
-      <c r="DD15" s="12"/>
-      <c r="DE15" s="13"/>
-    </row>
-    <row r="16" spans="1:109" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B16" s="22"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="12"/>
-      <c r="O16" s="12"/>
-      <c r="P16" s="12"/>
-      <c r="Q16" s="12"/>
-      <c r="R16" s="12"/>
-      <c r="S16" s="12"/>
-      <c r="T16" s="12"/>
-      <c r="U16" s="12"/>
-      <c r="V16" s="12"/>
-      <c r="W16" s="12"/>
-      <c r="X16" s="12"/>
-      <c r="Y16" s="12"/>
-      <c r="Z16" s="12"/>
-      <c r="AA16" s="12"/>
-      <c r="AB16" s="12"/>
-      <c r="AC16" s="12"/>
-      <c r="AD16" s="12"/>
-      <c r="AE16" s="12"/>
-      <c r="AF16" s="12"/>
-      <c r="AG16" s="12"/>
-      <c r="AH16" s="12"/>
-      <c r="AI16" s="12"/>
-      <c r="AJ16" s="12"/>
-      <c r="AK16" s="12"/>
-      <c r="AL16" s="12"/>
-      <c r="AM16" s="12"/>
-      <c r="AN16" s="12"/>
-      <c r="AO16" s="12"/>
-      <c r="AP16" s="12"/>
-      <c r="AQ16" s="12"/>
-      <c r="AR16" s="12"/>
-      <c r="AS16" s="12"/>
-      <c r="AT16" s="12"/>
-      <c r="AU16" s="12"/>
-      <c r="AV16" s="12"/>
-      <c r="AW16" s="12"/>
-      <c r="AX16" s="12"/>
-      <c r="AY16" s="12"/>
-      <c r="AZ16" s="12"/>
-      <c r="BA16" s="12"/>
-      <c r="BB16" s="12"/>
-      <c r="BC16" s="12"/>
-      <c r="BD16" s="12"/>
-      <c r="BE16" s="12"/>
-      <c r="BF16" s="12"/>
-      <c r="BG16" s="12"/>
-      <c r="BH16" s="12"/>
-      <c r="BI16" s="14"/>
-      <c r="BJ16" s="14"/>
-      <c r="BK16" s="14"/>
-      <c r="BL16" s="14"/>
-      <c r="BM16" s="14"/>
-      <c r="BN16" s="14"/>
-      <c r="BO16" s="12"/>
-      <c r="BP16" s="12"/>
-      <c r="BQ16" s="12"/>
-      <c r="BR16" s="12"/>
-      <c r="BS16" s="12"/>
-      <c r="BT16" s="12"/>
-      <c r="BU16" s="12"/>
-      <c r="BV16" s="12"/>
-      <c r="BW16" s="12"/>
-      <c r="BX16" s="12"/>
-      <c r="BY16" s="12"/>
-      <c r="BZ16" s="12"/>
-      <c r="CA16" s="12"/>
-      <c r="CB16" s="12"/>
-      <c r="CC16" s="12"/>
-      <c r="CD16" s="12"/>
-      <c r="CE16" s="12"/>
-      <c r="CF16" s="12"/>
-      <c r="CG16" s="12"/>
-      <c r="CH16" s="12"/>
-      <c r="CI16" s="12"/>
-      <c r="CJ16" s="12"/>
-      <c r="CK16" s="12"/>
-      <c r="CL16" s="12"/>
-      <c r="CM16" s="12"/>
-      <c r="CN16" s="12"/>
-      <c r="CO16" s="12"/>
-      <c r="CP16" s="12"/>
-      <c r="CQ16" s="12"/>
-      <c r="CR16" s="12"/>
-      <c r="CS16" s="12"/>
-      <c r="CT16" s="12"/>
-      <c r="CU16" s="12"/>
-      <c r="CV16" s="12"/>
-      <c r="CW16" s="12"/>
-      <c r="CX16" s="12"/>
-      <c r="CY16" s="12"/>
-      <c r="CZ16" s="12"/>
-      <c r="DA16" s="12"/>
-      <c r="DB16" s="12"/>
-      <c r="DC16" s="12"/>
-      <c r="DD16" s="12"/>
-      <c r="DE16" s="13"/>
-    </row>
-    <row r="17" spans="1:109" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" s="22"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="12"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="12"/>
-      <c r="M17" s="12"/>
-      <c r="N17" s="12"/>
-      <c r="O17" s="12"/>
-      <c r="P17" s="12"/>
-      <c r="Q17" s="12"/>
-      <c r="R17" s="12"/>
-      <c r="S17" s="12"/>
-      <c r="T17" s="12"/>
-      <c r="U17" s="12"/>
-      <c r="V17" s="12"/>
-      <c r="W17" s="12"/>
-      <c r="X17" s="12"/>
-      <c r="Y17" s="12"/>
-      <c r="Z17" s="12"/>
-      <c r="AA17" s="12"/>
-      <c r="AB17" s="12"/>
-      <c r="AC17" s="12"/>
-      <c r="AD17" s="12"/>
-      <c r="AE17" s="12"/>
-      <c r="AF17" s="12"/>
-      <c r="AG17" s="12"/>
-      <c r="AH17" s="12"/>
-      <c r="AI17" s="12"/>
-      <c r="AJ17" s="12"/>
-      <c r="AK17" s="12"/>
-      <c r="AL17" s="12"/>
-      <c r="AM17" s="12"/>
-      <c r="AN17" s="12"/>
-      <c r="AO17" s="12"/>
-      <c r="AP17" s="12"/>
-      <c r="AQ17" s="12"/>
-      <c r="AR17" s="12"/>
-      <c r="AS17" s="12"/>
-      <c r="AT17" s="12"/>
-      <c r="AU17" s="12"/>
-      <c r="AV17" s="12"/>
-      <c r="AW17" s="12"/>
-      <c r="AX17" s="12"/>
-      <c r="AY17" s="12"/>
-      <c r="AZ17" s="12"/>
-      <c r="BA17" s="12"/>
-      <c r="BB17" s="12"/>
-      <c r="BC17" s="12"/>
-      <c r="BD17" s="12"/>
-      <c r="BE17" s="12"/>
-      <c r="BF17" s="12"/>
-      <c r="BG17" s="12"/>
-      <c r="BH17" s="12"/>
-      <c r="BI17" s="12"/>
-      <c r="BJ17" s="12"/>
-      <c r="BK17" s="12"/>
-      <c r="BL17" s="12"/>
-      <c r="BM17" s="12"/>
-      <c r="BN17" s="12"/>
-      <c r="BO17" s="14"/>
-      <c r="BP17" s="14"/>
-      <c r="BQ17" s="14"/>
-      <c r="BR17" s="14"/>
-      <c r="BS17" s="14"/>
-      <c r="BT17" s="14"/>
-      <c r="BU17" s="14"/>
-      <c r="BV17" s="14"/>
-      <c r="BW17" s="14"/>
-      <c r="BX17" s="14"/>
-      <c r="BY17" s="14"/>
-      <c r="BZ17" s="14"/>
-      <c r="CA17" s="14"/>
-      <c r="CB17" s="14"/>
-      <c r="CC17" s="14"/>
-      <c r="CD17" s="14"/>
-      <c r="CE17" s="14"/>
-      <c r="CF17" s="14"/>
-      <c r="CG17" s="14"/>
-      <c r="CH17" s="14"/>
-      <c r="CI17" s="14"/>
-      <c r="CJ17" s="14"/>
-      <c r="CK17" s="14"/>
-      <c r="CL17" s="27"/>
-      <c r="CM17" s="12"/>
-      <c r="CN17" s="12"/>
-      <c r="CO17" s="12"/>
-      <c r="CP17" s="12"/>
-      <c r="CQ17" s="12"/>
-      <c r="CR17" s="12"/>
-      <c r="CS17" s="12"/>
-      <c r="CT17" s="12"/>
-      <c r="CU17" s="12"/>
-      <c r="CV17" s="12"/>
-      <c r="CW17" s="12"/>
-      <c r="CX17" s="12"/>
-      <c r="CY17" s="12"/>
-      <c r="CZ17" s="12"/>
-      <c r="DA17" s="12"/>
-      <c r="DB17" s="12"/>
-      <c r="DC17" s="12"/>
-      <c r="DD17" s="12"/>
-      <c r="DE17" s="13"/>
-    </row>
-    <row r="18" spans="1:109" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="B18" s="28"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="15"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="15"/>
-      <c r="M18" s="15"/>
-      <c r="N18" s="15"/>
-      <c r="O18" s="15"/>
-      <c r="P18" s="15"/>
-      <c r="Q18" s="15"/>
-      <c r="R18" s="15"/>
-      <c r="S18" s="15"/>
-      <c r="T18" s="15"/>
-      <c r="U18" s="15"/>
-      <c r="V18" s="15"/>
-      <c r="W18" s="15"/>
-      <c r="X18" s="15"/>
-      <c r="Y18" s="15"/>
-      <c r="Z18" s="15"/>
-      <c r="AA18" s="15"/>
-      <c r="AB18" s="15"/>
-      <c r="AC18" s="15"/>
-      <c r="AD18" s="15"/>
-      <c r="AE18" s="15"/>
-      <c r="AF18" s="15"/>
-      <c r="AG18" s="15"/>
-      <c r="AH18" s="15"/>
-      <c r="AI18" s="15"/>
-      <c r="AJ18" s="15"/>
-      <c r="AK18" s="15"/>
-      <c r="AL18" s="15"/>
-      <c r="AM18" s="15"/>
-      <c r="AN18" s="15"/>
-      <c r="AO18" s="15"/>
-      <c r="AP18" s="15"/>
-      <c r="AQ18" s="15"/>
-      <c r="AR18" s="15"/>
-      <c r="AS18" s="15"/>
-      <c r="AT18" s="15"/>
-      <c r="AU18" s="15"/>
-      <c r="AV18" s="15"/>
-      <c r="AW18" s="15"/>
-      <c r="AX18" s="15"/>
-      <c r="AY18" s="15"/>
-      <c r="AZ18" s="15"/>
-      <c r="BA18" s="15"/>
-      <c r="BB18" s="15"/>
-      <c r="BC18" s="15"/>
-      <c r="BD18" s="15"/>
-      <c r="BE18" s="15"/>
-      <c r="BF18" s="15"/>
-      <c r="BG18" s="15"/>
-      <c r="BH18" s="15"/>
-      <c r="BI18" s="15"/>
-      <c r="BJ18" s="15"/>
-      <c r="BK18" s="15"/>
-      <c r="BL18" s="15"/>
-      <c r="BM18" s="15"/>
-      <c r="BN18" s="15"/>
-      <c r="BO18" s="15"/>
-      <c r="BP18" s="15"/>
-      <c r="BQ18" s="15"/>
-      <c r="BR18" s="15"/>
-      <c r="BS18" s="15"/>
-      <c r="BT18" s="15"/>
-      <c r="BU18" s="15"/>
-      <c r="BV18" s="15"/>
-      <c r="BW18" s="15"/>
-      <c r="BX18" s="15"/>
-      <c r="BY18" s="15"/>
-      <c r="BZ18" s="15"/>
-      <c r="CA18" s="15"/>
-      <c r="CB18" s="15"/>
-      <c r="CC18" s="15"/>
-      <c r="CD18" s="15"/>
-      <c r="CE18" s="15"/>
-      <c r="CF18" s="15"/>
-      <c r="CG18" s="15"/>
-      <c r="CH18" s="15"/>
-      <c r="CI18" s="15"/>
-      <c r="CJ18" s="15"/>
-      <c r="CK18" s="15"/>
-      <c r="CL18" s="15"/>
-      <c r="CM18" s="15"/>
-      <c r="CN18" s="15"/>
-      <c r="CO18" s="15"/>
-      <c r="CP18" s="15"/>
-      <c r="CQ18" s="15"/>
-      <c r="CR18" s="15"/>
-      <c r="CS18" s="15"/>
-      <c r="CT18" s="15"/>
-      <c r="CU18" s="15"/>
-      <c r="CV18" s="15"/>
-      <c r="CW18" s="15"/>
-      <c r="CX18" s="15"/>
-      <c r="CY18" s="15"/>
-      <c r="CZ18" s="15"/>
-      <c r="DA18" s="15"/>
-      <c r="DB18" s="15"/>
-      <c r="DC18" s="15"/>
-      <c r="DD18" s="15"/>
-      <c r="DE18" s="29"/>
-    </row>
-    <row r="19" spans="1:109" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:109" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="1:109" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:109" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:109" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:109" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:109" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:109" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:109" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:109" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:109" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:109" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:109" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="CD15" s="13"/>
+    </row>
+    <row r="16" spans="1:82" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="28"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="15"/>
+      <c r="M16" s="15"/>
+      <c r="N16" s="15"/>
+      <c r="O16" s="15"/>
+      <c r="P16" s="15"/>
+      <c r="Q16" s="15"/>
+      <c r="R16" s="15"/>
+      <c r="S16" s="15"/>
+      <c r="T16" s="15"/>
+      <c r="U16" s="15"/>
+      <c r="V16" s="15"/>
+      <c r="W16" s="15"/>
+      <c r="X16" s="15"/>
+      <c r="Y16" s="15"/>
+      <c r="Z16" s="15"/>
+      <c r="AA16" s="15"/>
+      <c r="AB16" s="15"/>
+      <c r="AC16" s="15"/>
+      <c r="AD16" s="15"/>
+      <c r="AE16" s="15"/>
+      <c r="AF16" s="15"/>
+      <c r="AG16" s="15"/>
+      <c r="AH16" s="15"/>
+      <c r="AI16" s="15"/>
+      <c r="AJ16" s="15"/>
+      <c r="AK16" s="15"/>
+      <c r="AL16" s="15"/>
+      <c r="AM16" s="15"/>
+      <c r="AN16" s="15"/>
+      <c r="AO16" s="15"/>
+      <c r="AP16" s="15"/>
+      <c r="AQ16" s="15"/>
+      <c r="AR16" s="15"/>
+      <c r="AS16" s="15"/>
+      <c r="AT16" s="15"/>
+      <c r="AU16" s="15"/>
+      <c r="AV16" s="15"/>
+      <c r="AW16" s="15"/>
+      <c r="AX16" s="15"/>
+      <c r="AY16" s="15"/>
+      <c r="AZ16" s="15"/>
+      <c r="BA16" s="15"/>
+      <c r="BB16" s="15"/>
+      <c r="BC16" s="15"/>
+      <c r="BD16" s="15"/>
+      <c r="BE16" s="15"/>
+      <c r="BF16" s="15"/>
+      <c r="BG16" s="15"/>
+      <c r="BH16" s="15"/>
+      <c r="BI16" s="15"/>
+      <c r="BJ16" s="15"/>
+      <c r="BK16" s="15"/>
+      <c r="BL16" s="15"/>
+      <c r="BM16" s="15"/>
+      <c r="BN16" s="15"/>
+      <c r="BO16" s="15"/>
+      <c r="BP16" s="15"/>
+      <c r="BQ16" s="15"/>
+      <c r="BR16" s="15"/>
+      <c r="BS16" s="15"/>
+      <c r="BT16" s="15"/>
+      <c r="BU16" s="15"/>
+      <c r="BV16" s="15"/>
+      <c r="BW16" s="15"/>
+      <c r="BX16" s="15"/>
+      <c r="BY16" s="15"/>
+      <c r="BZ16" s="15"/>
+      <c r="CA16" s="15"/>
+      <c r="CB16" s="15"/>
+      <c r="CC16" s="15"/>
+      <c r="CD16" s="29"/>
+    </row>
+    <row r="17" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="27">
-    <mergeCell ref="CT1:CW1"/>
-    <mergeCell ref="CX1:DB1"/>
-    <mergeCell ref="DC1:DE1"/>
+  <mergeCells count="18">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="O1:S1"/>
+    <mergeCell ref="T1:W1"/>
+    <mergeCell ref="X1:AB1"/>
+    <mergeCell ref="AC1:AF1"/>
+    <mergeCell ref="AG1:AK1"/>
+    <mergeCell ref="AL1:AO1"/>
+    <mergeCell ref="AP1:AT1"/>
+    <mergeCell ref="AU1:AX1"/>
+    <mergeCell ref="AY1:BC1"/>
     <mergeCell ref="BV1:BY1"/>
     <mergeCell ref="BZ1:CD1"/>
-    <mergeCell ref="CE1:CG1"/>
-    <mergeCell ref="CH1:CK1"/>
-    <mergeCell ref="CL1:CP1"/>
-    <mergeCell ref="CQ1:CS1"/>
-    <mergeCell ref="BS1:BU1"/>
-    <mergeCell ref="Z1:AC1"/>
-    <mergeCell ref="AD1:AH1"/>
-    <mergeCell ref="AI1:AK1"/>
-    <mergeCell ref="AL1:AO1"/>
-    <mergeCell ref="AP1:AT1"/>
-    <mergeCell ref="AU1:AW1"/>
-    <mergeCell ref="AX1:BA1"/>
-    <mergeCell ref="BB1:BF1"/>
-    <mergeCell ref="BG1:BI1"/>
-    <mergeCell ref="BJ1:BM1"/>
-    <mergeCell ref="BN1:BR1"/>
-    <mergeCell ref="W1:Y1"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="R1:V1"/>
+    <mergeCell ref="BD1:BG1"/>
+    <mergeCell ref="BH1:BL1"/>
+    <mergeCell ref="BM1:BP1"/>
+    <mergeCell ref="BQ1:BU1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>